<commit_message>
9 paskaita - gridTask3
</commit_message>
<xml_diff>
--- a/HTML ir CSS/09 paskaita - 11.17 - Grid/grid.xlsx
+++ b/HTML ir CSS/09 paskaita - 11.17 - Grid/grid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Darbas\CodeAcademy\2022+\FEU3\praktika\HTML ir CSS\09 paskaita - 11.17 - Grid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D71186-1963-4C2B-BA59-D524CA4CD6A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B2AD40-FDE4-48C6-97BA-753AEA1B3521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,18 +35,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -63,9 +57,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -346,35 +338,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C1:D3"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="0.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" customWidth="1"/>
-    <col min="6" max="6" width="104.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="14" style="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="3:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="3:4" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="3:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C2:D3"/>
-  </mergeCells>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>